<commit_message>
Adding Multiple Product Test
</commit_message>
<xml_diff>
--- a/src/main/resources/configfile/testData.xlsx
+++ b/src/main/resources/configfile/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HousingMan\eclipse-workspace\FlipkartPomDD\src\main\resources\configfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480B1901-F552-43AD-874D-4773F03D9E33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72972E5-D777-4546-BE8D-B100FF113313}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3F98F14D-154F-4938-8298-748EB6362DA4}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>TestName</t>
   </si>
@@ -122,7 +122,10 @@
     <t>8553610403</t>
   </si>
   <si>
-    <t>f17890k</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>f1234567890k</t>
   </si>
 </sst>
 </file>
@@ -650,7 +653,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +698,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -704,7 +707,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>

</xml_diff>